<commit_message>
Codigos de generacion de graficas
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data SciLab/Simulacion/DataSimSciLab.xlsx
+++ b/comparisonFiles/Data SciLab/Simulacion/DataSimSciLab.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
   <si>
     <t>Controlador</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>auto</t>
-  </si>
-  <si>
-    <t>auto(ode45)</t>
   </si>
   <si>
     <t>BDF-newt</t>
@@ -576,7 +573,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +633,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -665,7 +662,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -694,7 +691,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
@@ -709,7 +706,7 @@
         <v>2.2761865000000001</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M4" s="18"/>
     </row>
@@ -756,7 +753,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
@@ -783,7 +780,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>21</v>
@@ -799,7 +796,7 @@
         <v>3.6471898999999999</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -816,7 +813,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>19</v>
@@ -874,7 +871,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>24</v>
@@ -904,7 +901,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>19</v>
@@ -961,7 +958,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>28</v>
@@ -991,7 +988,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
@@ -1020,7 +1017,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>19</v>
@@ -1047,7 +1044,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>11</v>
@@ -1091,7 +1088,7 @@
         <v>2.7858963999999999</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tablas de parametros continuos para la comparacion de simulacion
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data SciLab/Simulacion/DataSimSciLab.xlsx
+++ b/comparisonFiles/Data SciLab/Simulacion/DataSimSciLab.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
   <si>
     <t>Controlador</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>0.2,1,1</t>
-  </si>
-  <si>
-    <t>auto</t>
   </si>
   <si>
     <t>BDF-newt</t>
@@ -573,7 +570,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +630,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -662,7 +659,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -691,7 +688,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
@@ -706,7 +703,7 @@
         <v>2.2761865000000001</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M4" s="18"/>
     </row>
@@ -753,7 +750,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
@@ -780,7 +777,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>21</v>
@@ -796,7 +793,7 @@
         <v>3.6471898999999999</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -813,7 +810,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>19</v>
@@ -871,7 +868,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>24</v>
@@ -901,7 +898,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>19</v>
@@ -958,7 +955,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>28</v>
@@ -988,7 +985,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
@@ -1017,7 +1014,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>19</v>
@@ -1044,7 +1041,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>11</v>
@@ -1066,14 +1063,14 @@
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="14">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D17" s="14">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>36</v>
@@ -1088,7 +1085,7 @@
         <v>2.7858963999999999</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>